<commit_message>
Final Data Cleaning and Prep
hopefull ready for model building and testing
</commit_message>
<xml_diff>
--- a/0.RunningListOfObservationsAndActions.xlsx
+++ b/0.RunningListOfObservationsAndActions.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmhenn/Documents/GitHub/Incident-Management-Process-BPIC2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8DA2FC6-4811-064E-9C7F-DD09B94A7A52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637B3AB1-FBD4-C54F-BC55-CFB5B24E6DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="960" windowWidth="28040" windowHeight="17440" xr2:uid="{FB96DE96-92D8-F34D-AAC6-E6F764F376C1}"/>
+    <workbookView xWindow="39460" yWindow="780" windowWidth="33400" windowHeight="19640" xr2:uid="{FB96DE96-92D8-F34D-AAC6-E6F764F376C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Running Notes" sheetId="1" r:id="rId1"/>
     <sheet name="Field Definitions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="211">
   <si>
     <t>CI_Name_aff</t>
   </si>
@@ -658,17 +658,6 @@
         <family val="2"/>
       </rPr>
       <t>CI Name (CBy)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF00004D"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Configuration Item (CI) which caused the disruption of an ICT Service, this is what we call the "CausedBy CI". When an Operator resolves an Incident , the CausedBy CI must be registered before closing the Incident-record.</t>
     </r>
   </si>
   <si>
@@ -785,14 +774,365 @@
     <t>monitor missing values that may be removed due to other data cleaning (restriction of dates)</t>
   </si>
   <si>
-    <t>Real number (ℝ≥0) ZEROS (58.9%)</t>
+    <t>Configuration Item (CI) where a disruption is noticed (Affected CI)</t>
+  </si>
+  <si>
+    <t>Configuration Item (CI) which caused the disruption of an ICT Service, this is what we call the "CausedBy CI". When an Operator resolves an Incident , the CausedBy CI must be registered before closing the Incident-record.</t>
+  </si>
+  <si>
+    <t>Configuration Item (CI) which caused the disruption (CausedBy CI)</t>
+  </si>
+  <si>
+    <t>Top-level category of Affected CI</t>
+  </si>
+  <si>
+    <t>Top-level category of CausedBy CI</t>
+  </si>
+  <si>
+    <t>Second-level category of Affected CI</t>
+  </si>
+  <si>
+    <t>Second-level category of CausedBy CI</t>
+  </si>
+  <si>
+    <t>Date and time of incident closure</t>
+  </si>
+  <si>
+    <t>Classification of disruption type</t>
+  </si>
+  <si>
+    <t>Number of time the incident was reassigned</t>
+  </si>
+  <si>
+    <t>Number of Change Management records associated with the incident</t>
+  </si>
+  <si>
+    <t>Number of similar or related incidents (child records)</t>
+  </si>
+  <si>
+    <t>Number of updates or changes to the incident record</t>
+  </si>
+  <si>
+    <t>Time required to actively resolve the incident</t>
+  </si>
+  <si>
+    <t>Impact of the disruption to the customer</t>
+  </si>
+  <si>
+    <t>Unique identifier for each incident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Knowledge management article containing default attributes and questions for service desk analyst use </t>
+  </si>
+  <si>
+    <t>Date and time the incident was created</t>
+  </si>
+  <si>
+    <t>Priority derived from the Impact and Urgency values</t>
+  </si>
+  <si>
+    <t>Change record identifier (if only one change is related to the incident)</t>
+  </si>
+  <si>
+    <t>Interaction record identifier (if only one interact is related to the incident)</t>
+  </si>
+  <si>
+    <t>If the incident is re-opened within a short time of closure based on customer feedback, the date and time the incident was re-opened</t>
+  </si>
+  <si>
+    <t>Date and time the incident was resolved</t>
+  </si>
+  <si>
+    <t>Service component identifier for the Affected CI</t>
+  </si>
+  <si>
+    <t>Service component identifier for the CausedBy CI</t>
+  </si>
+  <si>
+    <t>Status of the incident</t>
+  </si>
+  <si>
+    <t>Indicates incident resolution urgency</t>
+  </si>
+  <si>
+    <t>Status for monitoring service levels</t>
+  </si>
+  <si>
+    <t>Grouping of types of incidents</t>
+  </si>
+  <si>
+    <t>Continuous, Real number (ℝ≥0), MISSING (97.4%)</t>
+  </si>
+  <si>
+    <t>Continuous, Real number (ℝ≥0) ZEROS (58.9%)</t>
+  </si>
+  <si>
+    <t>Real number (ℝ≥0), SKEWED</t>
+  </si>
+  <si>
+    <t>Profile reports as Categorical, however dtype is float64
+Continuous, Real number (ℝ≥0), MISSING (98.8%)</t>
+  </si>
+  <si>
+    <t>Monitor dtype in subsequent steps</t>
+  </si>
+  <si>
+    <t>Continuous, Real number (ℝ≥0)</t>
+  </si>
+  <si>
+    <t>Categorical, UNIQUE,
+HIGH CARDINALITY</t>
+  </si>
+  <si>
+    <t>Date 
+Minimum: 	2012-02-05 13:32:57
+Maximum: 	2014-03-31 17:24:49</t>
+  </si>
+  <si>
+    <t>Categorical, five levels</t>
+  </si>
+  <si>
+    <t>Categorical, MISSING (98.8%), 
+HIGH CARDINALITY</t>
+  </si>
+  <si>
+    <t>Date
+Minimum: 	2013-04-10 09:15:55
+Maximum: 	2014-03-31 16:21:15</t>
+  </si>
+  <si>
+    <t>Date
+Minimum: 	2013-10-01 06:45:36
+Maximum: 	2014-03-31 22:47:29</t>
+  </si>
+  <si>
+    <t>Categorical, two levels</t>
+  </si>
+  <si>
+    <t>Monitor "Work in Progress" as it might drop when restricting records to three months.</t>
+  </si>
+  <si>
+    <t>Topic Paper Description</t>
+  </si>
+  <si>
+    <t>Date
+Minimum: 2013-10-01 06:45:43
+Maximum: 2014-03-31 22:47:32</t>
+  </si>
+  <si>
+    <t>Date 
+Minimum: 2012-02-05 13:32:57
+Maximum: 2014-03-31 17:24:49</t>
+  </si>
+  <si>
+    <t>Date
+Minimum: 2013-04-10 09:15:55
+Maximum: 2014-03-31 16:21:15</t>
+  </si>
+  <si>
+    <t>Date
+Minimum: 2013-10-01 06:45:36
+Maximum: 2014-03-31 22:47:29</t>
+  </si>
+  <si>
+    <t>Categorical, CONSTANT value "closed"</t>
+  </si>
+  <si>
+    <t>Categorical, four levels</t>
+  </si>
+  <si>
+    <t>Categorical, 13 levels</t>
+  </si>
+  <si>
+    <t>Categorical, 14 levels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Categorical, 15 levels
+1.0% missing
+</t>
+  </si>
+  <si>
+    <t>Limit study to dates from 1 October 2013 through 31 March 2014 (Buffett et al, 2014)</t>
+  </si>
+  <si>
+    <t>The same level is interpreted differently by value_counts(), investigate</t>
+  </si>
+  <si>
+    <t>converting to string and using only the first character</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>drop field</t>
+  </si>
+  <si>
+    <t>2. Cleaning</t>
+  </si>
+  <si>
+    <t>records remain … drop them</t>
+  </si>
+  <si>
+    <t>Missing: 	1627
+Missing (%): 	4.4%</t>
+  </si>
+  <si>
+    <t>Missing values</t>
+  </si>
+  <si>
+    <t>Urgency, Impact, Priority</t>
+  </si>
+  <si>
+    <t>Highly Correlated with Priority being calculated from Urgency and Impact</t>
+  </si>
+  <si>
+    <t>drop Urgency and Impact</t>
+  </si>
+  <si>
+    <t>Met_SLA</t>
+  </si>
+  <si>
+    <t>Does not exist in the data set, need to calculate or set it by some business rule</t>
+  </si>
+  <si>
+    <t>Priority	SLA in Minutes	SLA in Hours	SLA in Days
+1 Very High 	240	4	0.16
+2 High	480	8	0.3
+3 Medium	1440	24	1
+4 Low	2880	48	2
+5 Very Low	5760	96	4</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>3. Create_SLAFail</t>
+  </si>
+  <si>
+    <t>3.Create SLAFail</t>
+  </si>
+  <si>
+    <t>SLAFail</t>
+  </si>
+  <si>
+    <t>CI_Type_aff, CI_Subtype_aff</t>
+  </si>
+  <si>
+    <t>CI_Type_Cby, CI_Subtype_Cby</t>
+  </si>
+  <si>
+    <t>Highly correlated</t>
+  </si>
+  <si>
+    <t>convert to strings: 
+1 Very High
+2 High
+3 Medium
+4 Low
+5 Very Low</t>
+  </si>
+  <si>
+    <t>aggregate by concatenation</t>
+  </si>
+  <si>
+    <t>integer data type</t>
+  </si>
+  <si>
+    <t>Close_Time, Open_Time, Reopen_Time, 
+Resolved_Time</t>
+  </si>
+  <si>
+    <t>Access to Day-of-Week and Hour-of-Day for these variables may introduce some insight</t>
+  </si>
+  <si>
+    <t>Create DayOfWeek and HourOfDay variables from the four time variables</t>
+  </si>
+  <si>
+    <t>4. Final Data Prep</t>
+  </si>
+  <si>
+    <t>An unbalanced data set with a 70/30 split, not rare events
+0    0.701261
+1    0.298739</t>
+  </si>
+  <si>
+    <t>create proportional stratified random sampled data sets for training and testing</t>
+  </si>
+  <si>
+    <t>drop records where missing</t>
+  </si>
+  <si>
+    <t>drop variable</t>
+  </si>
+  <si>
+    <t>see item 29</t>
+  </si>
+  <si>
+    <t>see other item</t>
+  </si>
+  <si>
+    <t>see item 35</t>
+  </si>
+  <si>
+    <t>information about 'shift' may be helpful</t>
+  </si>
+  <si>
+    <t>Create *Shift variables</t>
+  </si>
+  <si>
+    <t>concate with CI_Type_aff</t>
+  </si>
+  <si>
+    <t>concate with CI_Type_Cby</t>
+  </si>
+  <si>
+    <t>concate with CI_Type_aff for new var and drop</t>
+  </si>
+  <si>
+    <t>concate with CI_Subtype_aff for new var and drop</t>
+  </si>
+  <si>
+    <t>5. Model Building</t>
+  </si>
+  <si>
+    <t>concate for new var and drop</t>
+  </si>
+  <si>
+    <t>no action pre 5. Model Building</t>
+  </si>
+  <si>
+    <t>set missing values to 0</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>Reopen_Time has 33782 (95.9%) missing values
+Reopen_Time_DayOfWeek has 33782 (95.9%) missing values
+Reopen_Time_HourOfDay has 33782 (95.9%) missing values</t>
+  </si>
+  <si>
+    <t>Bin the variable to create a Reopened categorical variable with Yes and No levels</t>
+  </si>
+  <si>
+    <t>Close_Time, Open_Time, 
+Resolved_Time</t>
+  </si>
+  <si>
+    <t>Create DayOfWeek and HourOfDay variables from the three time variables</t>
+  </si>
+  <si>
+    <t>todo in 2. (in 4. remove code for creating DayOfWeek and HourOfDay)</t>
+  </si>
+  <si>
+    <t>todo in 4. remove code for creating Reopen_Time DayOfWeek and HourOfDay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -843,8 +1183,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -872,8 +1225,14 @@
         <fgColor rgb="FFED9ED9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -942,13 +1301,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1003,11 +1371,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
     <dxf>
       <font>
         <b val="0"/>
@@ -1122,48 +1517,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1197,6 +1550,51 @@
         </top>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1211,15 +1609,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E93A74F-7C8D-DD46-BCDF-7352698E0E8A}" name="Table1" displayName="Table1" ref="B1:I38" totalsRowShown="0">
-  <autoFilter ref="B1:I38" xr:uid="{94B46508-935A-624A-9E09-6A379551513A}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9E93A74F-7C8D-DD46-BCDF-7352698E0E8A}" name="Table1" displayName="Table1" ref="B1:K41" totalsRowShown="0">
+  <autoFilter ref="B1:K41" xr:uid="{94B46508-935A-624A-9E09-6A379551513A}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:K38">
     <sortCondition ref="D1:D38"/>
   </sortState>
-  <tableColumns count="8">
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{7B3D75FD-2DE0-3243-A0CE-9BB0DE1C4427}" name="Index"/>
     <tableColumn id="2" xr3:uid="{4D6348A7-DE37-7241-8305-E21D87FB7FC8}" name="Observation Step"/>
     <tableColumn id="3" xr3:uid="{9C551E42-6A37-5F47-B345-7737D300CC9E}" name="Variable"/>
+    <tableColumn id="9" xr3:uid="{D16613CD-49BA-C04E-BB42-30A366EEB647}" name="Topic Paper Description"/>
+    <tableColumn id="10" xr3:uid="{41D22B09-9FCF-D040-BCFF-E0E59D512542}" name="Description" dataDxfId="8">
+      <calculatedColumnFormula>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="4" xr3:uid="{48D7B998-E3A8-6C4F-9C07-1588BBCF1509}" name="Observation"/>
     <tableColumn id="5" xr3:uid="{309CC54E-D4DA-2C42-BE14-99E6906B6DD2}" name="Option"/>
     <tableColumn id="6" xr3:uid="{87EC899E-9CDB-EC41-93BE-8FE7CEC8E3E2}" name="Decision"/>
@@ -1231,10 +1633,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15B3AFE4-F064-404C-9320-7D1C3D3CF0B5}" name="Table2" displayName="Table2" ref="A3:E31" totalsRowShown="0" headerRowDxfId="4" dataDxfId="5" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15B3AFE4-F064-404C-9320-7D1C3D3CF0B5}" name="Table2" displayName="Table2" ref="A3:E31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A3:E31" xr:uid="{F1D69959-7817-7745-9481-CD0304322852}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F1B8F234-34DE-4D44-BDB0-CEED322ED8CF}" name="Variable" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{F1B8F234-34DE-4D44-BDB0-CEED322ED8CF}" name="Variable" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{6CE15344-8841-C843-A0E5-EBC0159BB940}" name="Description" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{F0D41033-E80D-5641-B27D-ADF699956AA9}" name="Column1" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{567D992E-5C23-1147-A248-42C5FF0B88A4}" name="Column2" dataDxfId="1"/>
@@ -1541,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F567229B-1C06-224D-9955-C66897FBAF2E}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1553,13 +1955,14 @@
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="26.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" customWidth="1"/>
-    <col min="6" max="6" width="30.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="26.83203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
+    <col min="8" max="8" width="30.1640625" customWidth="1"/>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+    <col min="10" max="10" width="27.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18">
+    <row r="1" spans="1:11" ht="18">
       <c r="A1" s="1"/>
       <c r="B1" t="s">
         <v>32</v>
@@ -1571,443 +1974,1109 @@
         <v>33</v>
       </c>
       <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H1" t="s">
         <v>92</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>93</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>94</v>
       </c>
-      <c r="H1" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18">
+    <row r="2" spans="1:11" ht="34">
       <c r="A2" s="1"/>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Status for monitoring service levels</v>
+      </c>
+      <c r="G2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" t="s">
         <v>96</v>
       </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="132" customHeight="1">
+      <c r="I2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="132" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="F3" s="22" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Grouping of types of incidents</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
         <v>98</v>
       </c>
-      <c r="F3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18">
+      <c r="I3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="51">
       <c r="A4" s="1"/>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18">
+      <c r="E4" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F4" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Configuration Item (CI) where a disruption is noticed (Affected CI)</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="51">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18">
+      <c r="E5" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Configuration Item (CI) which caused the disruption (CausedBy CI)</v>
+      </c>
+      <c r="G5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="51">
       <c r="A6" s="1"/>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18">
+      <c r="E6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Second-level category of Affected CI</v>
+      </c>
+      <c r="G6" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I6" t="s">
+        <v>199</v>
+      </c>
+      <c r="J6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="51">
       <c r="A7" s="1"/>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="51">
+      <c r="E7" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Second-level category of CausedBy CI</v>
+      </c>
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" t="s">
+        <v>197</v>
+      </c>
+      <c r="I7" t="s">
+        <v>199</v>
+      </c>
+      <c r="J7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="51">
       <c r="A8" s="1"/>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="F8" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Top-level category of Affected CI</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
         <v>101</v>
       </c>
-      <c r="F8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="51">
+      <c r="I8" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="51">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="F9" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Top-level category of CausedBy CI</v>
+      </c>
+      <c r="G9" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" t="s">
         <v>101</v>
       </c>
-      <c r="F9" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="51">
+      <c r="I9" t="s">
+        <v>198</v>
+      </c>
+      <c r="J9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="85">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
       </c>
-      <c r="E10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="51">
+      <c r="E10" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Date and time of incident closure</v>
+      </c>
+      <c r="G10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" t="s">
+        <v>158</v>
+      </c>
+      <c r="J10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="51">
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="51">
+      <c r="E11" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Classification of disruption type</v>
+      </c>
+      <c r="G11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="51">
       <c r="B12">
         <v>10.1</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="19"/>
+      <c r="F12" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Classification of disruption type</v>
+      </c>
+      <c r="G12" t="s">
+        <v>103</v>
+      </c>
+      <c r="H12" t="s">
         <v>104</v>
       </c>
-      <c r="F12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="17">
+      <c r="J12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="34">
       <c r="B13">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="17">
+      <c r="E13" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F13" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Number of time the incident was reassigned</v>
+      </c>
+      <c r="G13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="85">
       <c r="B14">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="17">
+      <c r="E14" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Number of Change Management records associated with the incident</v>
+      </c>
+      <c r="G14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H14" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" t="s">
+        <v>203</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="34">
       <c r="B15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="17">
+      <c r="E15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Number of similar or related incidents (child records)</v>
+      </c>
+      <c r="G15" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" t="s">
+        <v>203</v>
+      </c>
+      <c r="I15" t="s">
+        <v>203</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="34">
       <c r="B16">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" ht="17">
+      <c r="E16" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Number of updates or changes to the incident record</v>
+      </c>
+      <c r="G16" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="34">
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" ht="17">
+      <c r="E17" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="F17" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Time required to actively resolve the incident</v>
+      </c>
+      <c r="G17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="34">
       <c r="B18">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" ht="17">
+      <c r="E18" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F18" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Impact of the disruption to the customer</v>
+      </c>
+      <c r="G18" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" t="s">
+        <v>191</v>
+      </c>
+      <c r="J18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="34">
       <c r="B19">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="17">
+      <c r="E19" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="F19" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Unique identifier for each incident</v>
+      </c>
+      <c r="G19" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" t="s">
+        <v>190</v>
+      </c>
+      <c r="I19" t="s">
+        <v>190</v>
+      </c>
+      <c r="J19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="68">
       <c r="B20">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" ht="17">
+      <c r="E20" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v xml:space="preserve">Knowledge management article containing default attributes and questions for service desk analyst use </v>
+      </c>
+      <c r="G20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="85">
       <c r="B21">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" ht="17">
+      <c r="E21" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F21" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Date and time the incident was created</v>
+      </c>
+      <c r="G21" t="s">
+        <v>141</v>
+      </c>
+      <c r="H21" t="s">
+        <v>158</v>
+      </c>
+      <c r="J21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="34">
       <c r="B22">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" ht="17">
+      <c r="E22" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Priority derived from the Impact and Urgency values</v>
+      </c>
+      <c r="G22" t="s">
+        <v>142</v>
+      </c>
+      <c r="H22" t="s">
+        <v>193</v>
+      </c>
+      <c r="J22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="51">
       <c r="B23">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" ht="17">
+      <c r="E23" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="F23" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Change record identifier (if only one change is related to the incident)</v>
+      </c>
+      <c r="G23" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="51">
       <c r="B24">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" ht="17">
+      <c r="E24" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F24" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Interaction record identifier (if only one interact is related to the incident)</v>
+      </c>
+      <c r="G24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="85">
       <c r="B25">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" ht="17">
+      <c r="E25" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>If the incident is re-opened within a short time of closure based on customer feedback, the date and time the incident was re-opened</v>
+      </c>
+      <c r="G25" t="s">
+        <v>144</v>
+      </c>
+      <c r="H25" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" t="s">
+        <v>158</v>
+      </c>
+      <c r="J25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="85">
       <c r="B26">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" ht="17">
+      <c r="E26" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F26" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Date and time the incident was resolved</v>
+      </c>
+      <c r="G26" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" t="s">
+        <v>158</v>
+      </c>
+      <c r="I26" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="34">
       <c r="B27">
+        <v>24.1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" t="s">
         <v>25</v>
       </c>
-      <c r="C27" t="s">
-        <v>91</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="F27" s="23" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Date and time the incident was resolved</v>
+      </c>
+      <c r="G27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" t="s">
+        <v>189</v>
+      </c>
+      <c r="I27" t="s">
+        <v>189</v>
+      </c>
+      <c r="J27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="34">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" ht="17">
-      <c r="B28">
+      <c r="E28" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Service component identifier for the Affected CI</v>
+      </c>
+      <c r="G28" t="s">
+        <v>99</v>
+      </c>
+      <c r="J28" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="34">
+      <c r="B29">
         <v>26</v>
       </c>
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" ht="17">
-      <c r="B29">
+      <c r="E29" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Service component identifier for the CausedBy CI</v>
+      </c>
+      <c r="G29" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="51">
+      <c r="B30">
         <v>27</v>
       </c>
-      <c r="C29" t="s">
-        <v>91</v>
-      </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" ht="17">
-      <c r="B30">
+      <c r="E30" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F30" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Status of the incident</v>
+      </c>
+      <c r="G30" t="s">
+        <v>146</v>
+      </c>
+      <c r="H30" t="s">
+        <v>147</v>
+      </c>
+      <c r="I30" t="s">
+        <v>164</v>
+      </c>
+      <c r="J30" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="51">
+      <c r="B31">
         <v>28</v>
       </c>
-      <c r="C30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="2:4">
-      <c r="B31">
+      <c r="E31" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" s="21" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Indicates incident resolution urgency</v>
+      </c>
+      <c r="G31" t="s">
+        <v>159</v>
+      </c>
+      <c r="H31" t="s">
+        <v>160</v>
+      </c>
+      <c r="I31" t="s">
+        <v>161</v>
+      </c>
+      <c r="J31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="51">
+      <c r="B32">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="2:4">
-      <c r="B32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2">
+      <c r="C32" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" t="s">
+        <v>167</v>
+      </c>
+      <c r="F32" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G32" t="s">
+        <v>168</v>
+      </c>
+      <c r="H32" t="s">
+        <v>169</v>
+      </c>
+      <c r="I32" t="s">
+        <v>173</v>
+      </c>
+      <c r="J32" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="119">
       <c r="B33">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="2:2">
+      <c r="C33" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G33" t="s">
+        <v>171</v>
+      </c>
+      <c r="H33" t="s">
+        <v>172</v>
+      </c>
+      <c r="I33" t="s">
+        <v>173</v>
+      </c>
+      <c r="J33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="68">
       <c r="B34">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="2:2">
+      <c r="C34" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" t="s">
+        <v>176</v>
+      </c>
+      <c r="F34" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G34" t="s">
+        <v>187</v>
+      </c>
+      <c r="H34" t="s">
+        <v>188</v>
+      </c>
+      <c r="J34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="34">
       <c r="B35">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="2:2">
+      <c r="C35" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35" t="s">
+        <v>177</v>
+      </c>
+      <c r="F35" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G35" t="s">
+        <v>179</v>
+      </c>
+      <c r="H35" t="s">
+        <v>181</v>
+      </c>
+      <c r="I35" t="s">
+        <v>201</v>
+      </c>
+      <c r="J35" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="34">
       <c r="B36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="2:2">
+      <c r="C36" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" t="s">
+        <v>178</v>
+      </c>
+      <c r="F36" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G36" t="s">
+        <v>179</v>
+      </c>
+      <c r="H36" t="s">
+        <v>181</v>
+      </c>
+      <c r="I36" t="s">
+        <v>201</v>
+      </c>
+      <c r="J36" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="119">
       <c r="B37">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="2:2">
+      <c r="C37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>Priority derived from the Impact and Urgency values</v>
+      </c>
+      <c r="G37" t="s">
+        <v>182</v>
+      </c>
+      <c r="H37" t="s">
+        <v>180</v>
+      </c>
+      <c r="I37" t="s">
+        <v>173</v>
+      </c>
+      <c r="J37" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="153">
       <c r="B38">
         <v>36</v>
       </c>
+      <c r="C38" t="s">
+        <v>163</v>
+      </c>
+      <c r="D38" t="s">
+        <v>207</v>
+      </c>
+      <c r="F38" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G38" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" t="s">
+        <v>185</v>
+      </c>
+      <c r="I38" t="s">
+        <v>208</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>186</v>
+      </c>
+      <c r="K38" s="24" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="51">
+      <c r="C39" t="s">
+        <v>163</v>
+      </c>
+      <c r="D39" t="s">
+        <v>183</v>
+      </c>
+      <c r="F39" s="25" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G39" t="s">
+        <v>194</v>
+      </c>
+      <c r="H39" t="s">
+        <v>195</v>
+      </c>
+      <c r="I39" t="s">
+        <v>195</v>
+      </c>
+      <c r="J39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="136">
+      <c r="C40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="25" t="str">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>If the incident is re-opened within a short time of closure based on customer feedback, the date and time the incident was re-opened</v>
+      </c>
+      <c r="G40" t="s">
+        <v>205</v>
+      </c>
+      <c r="I40" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="F41" s="25" t="e">
+        <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
+        <v>#N/A</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2019,20 +3088,21 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="89" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="5" max="5" width="87.6640625" customWidth="1"/>
     <col min="8" max="8" width="66" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="34">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17">
@@ -2056,7 +3126,9 @@
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="C4" s="11" t="s">
         <v>68</v>
       </c>
@@ -2069,7 +3141,9 @@
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>133</v>
+      </c>
       <c r="C5" s="11" t="s">
         <v>52</v>
       </c>
@@ -2082,33 +3156,39 @@
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>105</v>
+      </c>
       <c r="C6" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="24">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="C7" s="15" t="s">
         <v>82</v>
       </c>
       <c r="D7" s="16"/>
-      <c r="E7" s="6" t="s">
-        <v>83</v>
+      <c r="E7" s="18" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
@@ -2121,9 +3201,11 @@
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="C9" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="6" t="s">
@@ -2134,7 +3216,9 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="C10" s="9" t="s">
         <v>36</v>
       </c>
@@ -2147,9 +3231,11 @@
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>109</v>
+      </c>
       <c r="C11" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="6" t="s">
@@ -2160,7 +3246,9 @@
       <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="C12" s="11" t="s">
         <v>62</v>
       </c>
@@ -2173,7 +3261,9 @@
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>113</v>
+      </c>
       <c r="C13" s="11" t="s">
         <v>66</v>
       </c>
@@ -2186,7 +3276,9 @@
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="4" t="s">
+        <v>114</v>
+      </c>
       <c r="C14" s="11" t="s">
         <v>70</v>
       </c>
@@ -2199,7 +3291,9 @@
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="C15" s="11" t="s">
         <v>78</v>
       </c>
@@ -2212,7 +3306,9 @@
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="C16" s="11" t="s">
         <v>76</v>
       </c>
@@ -2225,7 +3321,9 @@
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="C17" s="11" t="s">
         <v>72</v>
       </c>
@@ -2238,7 +3336,9 @@
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="C18" s="11" t="s">
         <v>64</v>
       </c>
@@ -2251,7 +3351,9 @@
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="C19" s="11" t="s">
         <v>46</v>
       </c>
@@ -2264,7 +3366,9 @@
       <c r="A20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="C20" s="11" t="s">
         <v>42</v>
       </c>
@@ -2280,7 +3384,9 @@
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="C21" s="11" t="s">
         <v>54</v>
       </c>
@@ -2293,7 +3399,9 @@
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="C22" s="11" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +3414,9 @@
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="C23" s="11" t="s">
         <v>50</v>
       </c>
@@ -2319,7 +3429,9 @@
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="C24" s="11" t="s">
         <v>80</v>
       </c>
@@ -2332,7 +3444,9 @@
       <c r="A25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="C25" s="11" t="s">
         <v>74</v>
       </c>
@@ -2341,11 +3455,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="24">
+    <row r="26" spans="1:8" ht="34">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="4"/>
+      <c r="B26" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="C26" s="11" t="s">
         <v>58</v>
       </c>
@@ -2358,7 +3474,9 @@
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="4"/>
+      <c r="B27" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="C27" s="11" t="s">
         <v>60</v>
       </c>
@@ -2371,7 +3489,9 @@
       <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="4"/>
+      <c r="B28" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="C28" s="9" t="s">
         <v>40</v>
       </c>
@@ -2384,20 +3504,24 @@
       <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="4"/>
+      <c r="B29" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="C29" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="17">
       <c r="A30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B30" s="4"/>
+      <c r="B30" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="C30" s="11" t="s">
         <v>44</v>
       </c>
@@ -2410,7 +3534,9 @@
       <c r="A31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="4"/>
+      <c r="B31" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="C31" s="11" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Closing out Data Prep
Hopefully have EDA, cleaning, and other data prep done
</commit_message>
<xml_diff>
--- a/0.RunningListOfObservationsAndActions.xlsx
+++ b/0.RunningListOfObservationsAndActions.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmhenn/Documents/GitHub/Incident-Management-Process-BPIC2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637B3AB1-FBD4-C54F-BC55-CFB5B24E6DE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AA52A6-DB19-C74F-99E2-3437345BB522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39460" yWindow="780" windowWidth="33400" windowHeight="19640" xr2:uid="{FB96DE96-92D8-F34D-AAC6-E6F764F376C1}"/>
+    <workbookView xWindow="9400" yWindow="460" windowWidth="29000" windowHeight="23540" activeTab="4" xr2:uid="{FB96DE96-92D8-F34D-AAC6-E6F764F376C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Running Notes" sheetId="1" r:id="rId1"/>
-    <sheet name="Field Definitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Encoders" sheetId="3" r:id="rId2"/>
+    <sheet name="Feature Selections" sheetId="4" r:id="rId3"/>
+    <sheet name="Field Definitions" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="264">
   <si>
     <t>CI_Name_aff</t>
   </si>
@@ -1122,17 +1125,240 @@
     <t>Create DayOfWeek and HourOfDay variables from the three time variables</t>
   </si>
   <si>
-    <t>todo in 2. (in 4. remove code for creating DayOfWeek and HourOfDay)</t>
-  </si>
-  <si>
-    <t>todo in 4. remove code for creating Reopen_Time DayOfWeek and HourOfDay</t>
+    <t>set missing values to "Not Applicable"</t>
+  </si>
+  <si>
+    <t>[2]</t>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t> encoder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t> encoder_list:...</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.basen.BaseNEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.binary.BinaryEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.cat_boost.CatBoostEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.hashing.HashingEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.helmert.HelmertEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.james_stein.JamesSteinEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.one_hot.OneHotEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.leave_one_out.LeaveOneOutEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.m_estimate.MEstimateEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.ordinal.OrdinalEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.polynomial.PolynomialEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.sum_coding.SumEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.target_encoder.TargetEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>&lt;class 'category_encoders.woe.WOEEncoder'&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t>for</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> encoder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> encoder_list:...</t>
+    </r>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>category_encoders.woe.WOEEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.binary.BinaryEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.leave_one_out.LeaveOneOutEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.polynomial.PolynomialEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.sum_coding.SumEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.one_hot.OneHotEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.basen.BaseNEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.ordinal.OrdinalEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.target_encoder.TargetEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.m_estimate.MEstimateEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.cat_boost.CatBoostEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.helmert.HelmertEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.hashing.HashingEncoder</t>
+  </si>
+  <si>
+    <t>category_encoders.james_stein.JamesSteinEncoder</t>
+  </si>
+  <si>
+    <t>5.z Test Encoders SLAFail LogReg</t>
+  </si>
+  <si>
+    <t>RandomForestClassifier results</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Logistic Regression</t>
+  </si>
+  <si>
+    <t>RFE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'CI_Name_aff'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Count_Related_Changes'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Count_Related_Interactions'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'KM_number'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Open_Time_DayOfWeek'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Impact'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Open_Time_HourOfDay'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Count_Related_Incidents'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'CI_TypeSubType_aff'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Urgency'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'Service_Component_WBS_aff'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> True</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> False</t>
+  </si>
+  <si>
+    <t>skb</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1196,8 +1422,26 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1223,12 +1467,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFED9ED9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1316,7 +1554,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1389,20 +1627,35 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -1593,6 +1846,85 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial Unicode MS"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
@@ -1619,7 +1951,7 @@
     <tableColumn id="2" xr3:uid="{4D6348A7-DE37-7241-8305-E21D87FB7FC8}" name="Observation Step"/>
     <tableColumn id="3" xr3:uid="{9C551E42-6A37-5F47-B345-7737D300CC9E}" name="Variable"/>
     <tableColumn id="9" xr3:uid="{D16613CD-49BA-C04E-BB42-30A366EEB647}" name="Topic Paper Description"/>
-    <tableColumn id="10" xr3:uid="{41D22B09-9FCF-D040-BCFF-E0E59D512542}" name="Description" dataDxfId="8">
+    <tableColumn id="10" xr3:uid="{41D22B09-9FCF-D040-BCFF-E0E59D512542}" name="Description" dataDxfId="14">
       <calculatedColumnFormula>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{48D7B998-E3A8-6C4F-9C07-1588BBCF1509}" name="Observation"/>
@@ -1633,6 +1965,66 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7CB8C393-A66C-4B45-AE8F-9EFB88E851E4}" name="Table3" displayName="Table3" ref="A4:C32" totalsRowShown="0">
+  <autoFilter ref="A4:C32" xr:uid="{0A53DBBE-635D-8441-BFD2-D7F9CC23F1E5}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{69E4703F-93EC-D346-8768-C08AA00E8DD0}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{002BE885-E761-8C48-8656-CB560703C9B5}" name="Column2" dataDxfId="13">
+      <calculatedColumnFormula>IFERROR(ROUND(A6,6),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{5596A612-D95E-2D46-BFF4-D406F6597E5A}" name="Column4" dataDxfId="12">
+      <calculatedColumnFormula>IFERROR(LEFT(RIGHT(A5,LEN(A5)-FIND("'",A5,8)),LEN(A5)-10),"")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{D3642F96-DCF6-0B4C-BF3E-806EC724CD39}" name="Table4" displayName="Table4" ref="E4:F31" totalsRowShown="0">
+  <autoFilter ref="E4:F31" xr:uid="{2FB0F202-EBDB-5D4D-B765-4E375F98A822}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E5:F31">
+    <sortCondition ref="E4:E31"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C708B620-3E63-AB43-95CC-5433551D6FDC}" name="Column2"/>
+    <tableColumn id="2" xr3:uid="{CA1C0868-ED2E-2944-8F3B-F8D068C477A9}" name="Column4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A2A0590-422E-8D47-B361-0954A29A8E07}" name="Table6" displayName="Table6" ref="A40:C68" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="A40:C68" xr:uid="{98B75448-2946-4E46-9CD6-39DDA41B8F78}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{BC1E53AF-D25D-AF45-B08A-71F8F0D86946}" name="Column1" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0969227F-04C5-CD4C-9569-BBCC5986633D}" name="Column2" dataDxfId="9">
+      <calculatedColumnFormula>IFERROR(ROUND(A42,6),"")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{49A6A201-275C-7C41-8384-C38A3514A7E5}" name="Column3" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(LEFT(RIGHT(A41,LEN(A41)-FIND("'",A41,8)),LEN(A41)-10),"")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BFDCCA1F-E576-BE4F-AA28-85F02E867175}" name="Table7" displayName="Table7" ref="E40:F67" totalsRowShown="0">
+  <autoFilter ref="E40:F67" xr:uid="{E3DFB259-5FDE-CA4D-8DFB-6E893E7430C0}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E41:F67">
+    <sortCondition ref="E40:E67"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{70225ED6-4EBA-BA45-88BF-DE78B29F6418}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{DF54C89B-2046-1345-8CDB-EC69D275CDC7}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{15B3AFE4-F064-404C-9320-7D1C3D3CF0B5}" name="Table2" displayName="Table2" ref="A3:E31" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6" tableBorderDxfId="5">
   <autoFilter ref="A3:E31" xr:uid="{F1D69959-7817-7745-9481-CD0304322852}"/>
   <tableColumns count="5">
@@ -1945,8 +2337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F567229B-1C06-224D-9955-C66897FBAF2E}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2362,12 +2754,10 @@
       <c r="I14" t="s">
         <v>203</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="K14" s="24" t="s">
-        <v>204</v>
-      </c>
+      <c r="K14" s="26"/>
     </row>
     <row r="15" spans="1:11" ht="34">
       <c r="B15">
@@ -2395,12 +2785,10 @@
       <c r="I15" t="s">
         <v>203</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="K15" s="24" t="s">
-        <v>204</v>
-      </c>
+      <c r="K15" s="26"/>
     </row>
     <row r="16" spans="1:11" ht="34">
       <c r="B16">
@@ -2422,11 +2810,17 @@
       <c r="G16" t="s">
         <v>136</v>
       </c>
-      <c r="J16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" ht="34">
+      <c r="H16" t="s">
+        <v>203</v>
+      </c>
+      <c r="I16" t="s">
+        <v>203</v>
+      </c>
+      <c r="J16" s="26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="34">
       <c r="B17">
         <v>15</v>
       </c>
@@ -2450,7 +2844,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="34">
+    <row r="18" spans="2:11" ht="34">
       <c r="B18">
         <v>16</v>
       </c>
@@ -2477,7 +2871,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="34">
+    <row r="19" spans="2:11" ht="34">
       <c r="B19">
         <v>17</v>
       </c>
@@ -2507,7 +2901,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="68">
+    <row r="20" spans="2:11" ht="68">
       <c r="B20">
         <v>18</v>
       </c>
@@ -2531,7 +2925,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="85">
+    <row r="21" spans="2:11" ht="85">
       <c r="B21">
         <v>19</v>
       </c>
@@ -2558,7 +2952,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="34">
+    <row r="22" spans="2:11" ht="34">
       <c r="B22">
         <v>20</v>
       </c>
@@ -2585,7 +2979,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="51">
+    <row r="23" spans="2:11" ht="51">
       <c r="B23">
         <v>21</v>
       </c>
@@ -2605,11 +2999,17 @@
       <c r="G23" t="s">
         <v>143</v>
       </c>
+      <c r="H23" t="s">
+        <v>209</v>
+      </c>
       <c r="J23" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" ht="51">
+        <v>163</v>
+      </c>
+      <c r="K23" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="51">
       <c r="B24">
         <v>22</v>
       </c>
@@ -2633,7 +3033,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="85">
+    <row r="25" spans="2:11" ht="85">
       <c r="B25">
         <v>23</v>
       </c>
@@ -2663,7 +3063,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="85">
+    <row r="26" spans="2:11" ht="85">
       <c r="B26">
         <v>24</v>
       </c>
@@ -2693,7 +3093,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="34">
+    <row r="27" spans="2:11" ht="34">
       <c r="B27">
         <v>24.1</v>
       </c>
@@ -2723,7 +3123,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="34">
+    <row r="28" spans="2:11" ht="34">
       <c r="B28">
         <v>25</v>
       </c>
@@ -2747,7 +3147,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="34">
+    <row r="29" spans="2:11" ht="34">
       <c r="B29">
         <v>26</v>
       </c>
@@ -2771,7 +3171,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="51">
+    <row r="30" spans="2:11" ht="51">
       <c r="B30">
         <v>27</v>
       </c>
@@ -2801,7 +3201,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="51">
+    <row r="31" spans="2:11" ht="51">
       <c r="B31">
         <v>28</v>
       </c>
@@ -2831,7 +3231,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="51">
+    <row r="32" spans="2:11" ht="51">
       <c r="B32">
         <v>29</v>
       </c>
@@ -2990,7 +3390,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="153">
+    <row r="38" spans="2:11" ht="68">
       <c r="B38">
         <v>36</v>
       </c>
@@ -3013,12 +3413,10 @@
       <c r="I38" t="s">
         <v>208</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="J38" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="K38" s="24" t="s">
-        <v>210</v>
-      </c>
+      <c r="K38" s="26"/>
     </row>
     <row r="39" spans="2:11" ht="51">
       <c r="C39" t="s">
@@ -3027,7 +3425,7 @@
       <c r="D39" t="s">
         <v>183</v>
       </c>
-      <c r="F39" s="25" t="e">
+      <c r="F39" s="24" t="e">
         <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
         <v>#N/A</v>
       </c>
@@ -3051,25 +3449,23 @@
       <c r="D40" t="s">
         <v>19</v>
       </c>
-      <c r="F40" s="25" t="str">
+      <c r="F40" s="24" t="str">
         <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
         <v>If the incident is re-opened within a short time of closure based on customer feedback, the date and time the incident was re-opened</v>
       </c>
       <c r="G40" t="s">
         <v>205</v>
       </c>
-      <c r="I40" s="26" t="s">
+      <c r="I40" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="J40" s="24" t="s">
+      <c r="J40" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="K40" s="24" t="s">
-        <v>209</v>
-      </c>
+      <c r="K40" s="26"/>
     </row>
     <row r="41" spans="2:11">
-      <c r="F41" s="25" t="e">
+      <c r="F41" s="24" t="e">
         <f>INDEX(Table2[],MATCH(Table1[[#This Row],[Variable]],Table2[Variable],0),2)</f>
         <v>#N/A</v>
       </c>
@@ -3084,6 +3480,1393 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F94A1FA-A4DA-7A4A-A91E-F7469C027059}">
+  <dimension ref="A1:F68"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="72.5" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="76.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
+    <col min="6" max="6" width="57.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="34">
+      <c r="E1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="34">
+      <c r="A3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17">
+      <c r="A5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B5" s="29">
+        <f t="shared" ref="B5:B32" si="0">IFERROR(ROUND(A6,6),"")</f>
+        <v>0.64527800000000002</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" ref="C5:C32" si="1">IFERROR(LEFT(RIGHT(A5,LEN(A5)-FIND("'",A5,8)),LEN(A5)-10),"")</f>
+        <v>category_encoders.basen.BaseNEncoder</v>
+      </c>
+      <c r="E5">
+        <v>0.63540474954414405</v>
+      </c>
+      <c r="F5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17">
+      <c r="A6">
+        <v>0.64527773504971897</v>
+      </c>
+      <c r="B6" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E6">
+        <v>0.64120175664123003</v>
+      </c>
+      <c r="F6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17">
+      <c r="A7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64120200000000005</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.binary.BinaryEncoder</v>
+      </c>
+      <c r="E7">
+        <v>0.64329955909442404</v>
+      </c>
+      <c r="F7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17">
+      <c r="A8">
+        <v>0.64120175664123003</v>
+      </c>
+      <c r="B8" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E8">
+        <v>0.64354395351273697</v>
+      </c>
+      <c r="F8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64841499999999996</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.cat_boost.CatBoostEncoder</v>
+      </c>
+      <c r="E9">
+        <v>0.644714208966917</v>
+      </c>
+      <c r="F9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17">
+      <c r="A10">
+        <v>0.64841486617988298</v>
+      </c>
+      <c r="B10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E10">
+        <v>0.64514509108972395</v>
+      </c>
+      <c r="F10" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17">
+      <c r="A11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64926600000000001</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.hashing.HashingEncoder</v>
+      </c>
+      <c r="E11">
+        <v>0.64527773504971897</v>
+      </c>
+      <c r="F11" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17">
+      <c r="A12">
+        <v>0.64926642150899505</v>
+      </c>
+      <c r="B12" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E12">
+        <v>0.64695355308511004</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17">
+      <c r="A13" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64885899999999996</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.helmert.HelmertEncoder</v>
+      </c>
+      <c r="E13">
+        <v>0.64808639790316303</v>
+      </c>
+      <c r="F13" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17">
+      <c r="A14">
+        <v>0.64885852511189002</v>
+      </c>
+      <c r="B14" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E14">
+        <v>0.64831242315409499</v>
+      </c>
+      <c r="F14" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17">
+      <c r="A15" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.65259100000000003</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.james_stein.JamesSteinEncoder</v>
+      </c>
+      <c r="E15">
+        <v>0.64841486617988298</v>
+      </c>
+      <c r="F15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17">
+      <c r="A16">
+        <v>0.65259114948054298</v>
+      </c>
+      <c r="B16" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E16">
+        <v>0.64885852511189002</v>
+      </c>
+      <c r="F16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64514499999999997</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.one_hot.OneHotEncoder</v>
+      </c>
+      <c r="E17">
+        <v>0.64926642150899505</v>
+      </c>
+      <c r="F17" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17">
+      <c r="A18">
+        <v>0.64514509108972395</v>
+      </c>
+      <c r="B18" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="E18">
+        <v>0.65259114948054298</v>
+      </c>
+      <c r="F18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17">
+      <c r="A19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B19" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64329999999999998</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.leave_one_out.LeaveOneOutEncoder</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17">
+      <c r="A20">
+        <v>0.64329955909442404</v>
+      </c>
+      <c r="B20" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17">
+      <c r="A21" t="s">
+        <v>220</v>
+      </c>
+      <c r="B21" s="29">
+        <f t="shared" si="0"/>
+        <v>0.648312</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.m_estimate.MEstimateEncoder</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17">
+      <c r="A22">
+        <v>0.64831242315409499</v>
+      </c>
+      <c r="B22" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17">
+      <c r="A23" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64695400000000003</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.ordinal.OrdinalEncoder</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17">
+      <c r="A24">
+        <v>0.64695355308511004</v>
+      </c>
+      <c r="B24" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17">
+      <c r="A25" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="29">
+        <f t="shared" si="0"/>
+        <v>0.643544</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.polynomial.PolynomialEncoder</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17">
+      <c r="A26">
+        <v>0.64354395351273697</v>
+      </c>
+      <c r="B26" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17">
+      <c r="A27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B27" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64471400000000001</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.sum_coding.SumEncoder</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17">
+      <c r="A28">
+        <v>0.644714208966917</v>
+      </c>
+      <c r="B28" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17">
+      <c r="A29" t="s">
+        <v>224</v>
+      </c>
+      <c r="B29" s="29">
+        <f t="shared" si="0"/>
+        <v>0.64808600000000005</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.target_encoder.TargetEncoder</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17">
+      <c r="A30">
+        <v>0.64808639790316303</v>
+      </c>
+      <c r="B30" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17">
+      <c r="A31" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="29">
+        <f t="shared" si="0"/>
+        <v>0.635405</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="1"/>
+        <v>category_encoders.woe.WOEEncoder</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17">
+      <c r="A32">
+        <v>0.63540474954414405</v>
+      </c>
+      <c r="B32" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17">
+      <c r="A39" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17">
+      <c r="A41" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B41" s="30">
+        <f t="shared" ref="B41:B68" si="2">IFERROR(ROUND(A42,6),"")</f>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C41" s="28" t="str">
+        <f t="shared" ref="C41:C68" si="3">IFERROR(LEFT(RIGHT(A41,LEN(A41)-FIND("'",A41,8)),LEN(A41)-10),"")</f>
+        <v>category_encoders.basen.BaseNEncoder</v>
+      </c>
+      <c r="E41">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F41" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17">
+      <c r="A42" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B42" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C42" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E42">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F42" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17">
+      <c r="A43" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B43" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C43" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.binary.BinaryEncoder</v>
+      </c>
+      <c r="E43">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F43" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17">
+      <c r="A44" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B44" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C44" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E44">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F44" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17">
+      <c r="A45" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B45" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C45" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.cat_boost.CatBoostEncoder</v>
+      </c>
+      <c r="E45">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F45" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17">
+      <c r="A46" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B46" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C46" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E46">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F46" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17">
+      <c r="A47" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B47" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C47" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.hashing.HashingEncoder</v>
+      </c>
+      <c r="E47">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F47" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17">
+      <c r="A48" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B48" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C48" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E48">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F48" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="17">
+      <c r="A49" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C49" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.helmert.HelmertEncoder</v>
+      </c>
+      <c r="E49">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="17">
+      <c r="A50" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B50" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C50" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E50">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F50" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17">
+      <c r="A51" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B51" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C51" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.james_stein.JamesSteinEncoder</v>
+      </c>
+      <c r="E51">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F51" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17">
+      <c r="A52" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B52" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C52" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E52">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F52" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="17">
+      <c r="A53" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B53" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C53" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.one_hot.OneHotEncoder</v>
+      </c>
+      <c r="E53">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F53" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="17">
+      <c r="A54" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B54" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C54" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E54">
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="F54" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="17">
+      <c r="A55" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B55" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C55" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.leave_one_out.LeaveOneOutEncoder</v>
+      </c>
+      <c r="E55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F55" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17">
+      <c r="A56" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B56" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C56" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E56" t="s">
+        <v>244</v>
+      </c>
+      <c r="F56" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="17">
+      <c r="A57" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B57" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C57" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.m_estimate.MEstimateEncoder</v>
+      </c>
+      <c r="E57" t="s">
+        <v>244</v>
+      </c>
+      <c r="F57" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="17">
+      <c r="A58" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B58" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C58" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E58" t="s">
+        <v>244</v>
+      </c>
+      <c r="F58" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="17">
+      <c r="A59" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B59" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C59" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.ordinal.OrdinalEncoder</v>
+      </c>
+      <c r="E59" t="s">
+        <v>244</v>
+      </c>
+      <c r="F59" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="17">
+      <c r="A60" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B60" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C60" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E60" t="s">
+        <v>244</v>
+      </c>
+      <c r="F60" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="17">
+      <c r="A61" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="B61" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C61" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.polynomial.PolynomialEncoder</v>
+      </c>
+      <c r="E61" t="s">
+        <v>244</v>
+      </c>
+      <c r="F61" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="17">
+      <c r="A62" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B62" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C62" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E62" t="s">
+        <v>244</v>
+      </c>
+      <c r="F62" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="17">
+      <c r="A63" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B63" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C63" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.sum_coding.SumEncoder</v>
+      </c>
+      <c r="E63" t="s">
+        <v>244</v>
+      </c>
+      <c r="F63" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17">
+      <c r="A64" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B64" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C64" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E64" t="s">
+        <v>244</v>
+      </c>
+      <c r="F64" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="17">
+      <c r="A65" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="B65" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C65" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.target_encoder.TargetEncoder</v>
+      </c>
+      <c r="E65" t="s">
+        <v>244</v>
+      </c>
+      <c r="F65" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17">
+      <c r="A66" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B66" s="30" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C66" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E66" t="s">
+        <v>244</v>
+      </c>
+      <c r="F66" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="17">
+      <c r="A67" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="B67" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65664199999999995</v>
+      </c>
+      <c r="C67" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v>category_encoders.woe.WOEEncoder</v>
+      </c>
+      <c r="E67" t="s">
+        <v>244</v>
+      </c>
+      <c r="F67" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17">
+      <c r="A68" s="28">
+        <v>0.65664176497871896</v>
+      </c>
+      <c r="B68" s="30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="C68" s="28" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="4">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6ABCD42-C9AE-9443-A5B9-A0E03BC995D4}">
+  <dimension ref="A2:E30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.83203125" customWidth="1"/>
+    <col min="3" max="3" width="48.5" customWidth="1"/>
+    <col min="5" max="5" width="50" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="17">
+      <c r="A2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>249</v>
+      </c>
+      <c r="C6" t="s">
+        <v>258</v>
+      </c>
+      <c r="E6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C9" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="19">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="19">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C11" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="19">
+      <c r="A12" s="1">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>256</v>
+      </c>
+      <c r="C13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="19">
+      <c r="A14" s="1">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17">
+      <c r="A17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17">
+      <c r="A18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B18" t="s">
+        <v>262</v>
+      </c>
+      <c r="C18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18">
+      <c r="A19" s="31">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C19">
+        <v>336759.156621136</v>
+      </c>
+      <c r="E19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18">
+      <c r="A20" s="31">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>257</v>
+      </c>
+      <c r="C20">
+        <v>7218.3088601136997</v>
+      </c>
+      <c r="E20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="A21" s="31">
+        <v>5.63748088766366E-175</v>
+      </c>
+      <c r="B21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C21">
+        <v>795.31308248515495</v>
+      </c>
+      <c r="E21" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18">
+      <c r="A22" s="31">
+        <v>2.1564336059340999E-40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>249</v>
+      </c>
+      <c r="C22">
+        <v>177.03084704198599</v>
+      </c>
+      <c r="E22" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18">
+      <c r="A23" s="31">
+        <v>3.5416230913176899E-16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>253</v>
+      </c>
+      <c r="C23">
+        <v>66.4760970341204</v>
+      </c>
+      <c r="E23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18">
+      <c r="A24" s="31">
+        <v>1.54275383171003E-12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24">
+        <v>49.9932550800809</v>
+      </c>
+      <c r="E24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18">
+      <c r="A25" s="31">
+        <v>5.8679012816361099E-11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>251</v>
+      </c>
+      <c r="C25">
+        <v>42.864053976993098</v>
+      </c>
+      <c r="E25" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="18">
+      <c r="A26" s="31">
+        <v>0.103014928920586</v>
+      </c>
+      <c r="B26" t="s">
+        <v>256</v>
+      </c>
+      <c r="C26">
+        <v>2.65823589811207</v>
+      </c>
+      <c r="E26" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="18">
+      <c r="A27" s="31">
+        <v>0.19984243902814899</v>
+      </c>
+      <c r="B27" t="s">
+        <v>255</v>
+      </c>
+      <c r="C27">
+        <v>1.64352551443894</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="18">
+      <c r="A28" s="31">
+        <v>0.34426205477432498</v>
+      </c>
+      <c r="B28" t="s">
+        <v>252</v>
+      </c>
+      <c r="C28">
+        <v>0.89449518777260395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18">
+      <c r="A29" s="31">
+        <v>0.84284964393070405</v>
+      </c>
+      <c r="B29" t="s">
+        <v>248</v>
+      </c>
+      <c r="C29">
+        <v>3.9302974044397199E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="17"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71AE3FF-6B2A-3845-AAF4-2F157B259FB5}">
   <dimension ref="A1:H31"/>
   <sheetViews>
@@ -3552,4 +5335,18 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD804D-D4BC-DF4B-B369-C04D16475947}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
mostly analysis of various categorical encoders
</commit_message>
<xml_diff>
--- a/0.RunningListOfObservationsAndActions.xlsx
+++ b/0.RunningListOfObservationsAndActions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cmhenn/Documents/GitHub/Incident-Management-Process-BPIC2014/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AA52A6-DB19-C74F-99E2-3437345BB522}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDA6520-AAB0-E545-82EC-C688660BC842}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9400" yWindow="460" windowWidth="29000" windowHeight="23540" activeTab="4" xr2:uid="{FB96DE96-92D8-F34D-AAC6-E6F764F376C1}"/>
+    <workbookView xWindow="2480" yWindow="2860" windowWidth="29000" windowHeight="17560" activeTab="1" xr2:uid="{FB96DE96-92D8-F34D-AAC6-E6F764F376C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Running Notes" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="266">
   <si>
     <t>CI_Name_aff</t>
   </si>
@@ -1350,13 +1350,19 @@
   <si>
     <t>score</t>
   </si>
+  <si>
+    <t>&lt;class 'category_encoders.backward_difference.BackwardDifferenceEncoder'&gt;</t>
+  </si>
+  <si>
+    <t>category_encoders.backward_difference.BackwardDifferenceEncoder</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1648,7 +1654,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1995,8 +2001,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A2A0590-422E-8D47-B361-0954A29A8E07}" name="Table6" displayName="Table6" ref="A40:C68" totalsRowShown="0" dataDxfId="11">
-  <autoFilter ref="A40:C68" xr:uid="{98B75448-2946-4E46-9CD6-39DDA41B8F78}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{2A2A0590-422E-8D47-B361-0954A29A8E07}" name="Table6" displayName="Table6" ref="A40:C69" totalsRowShown="0" dataDxfId="11">
+  <autoFilter ref="A40:C69" xr:uid="{98B75448-2946-4E46-9CD6-39DDA41B8F78}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{BC1E53AF-D25D-AF45-B08A-71F8F0D86946}" name="Column1" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{0969227F-04C5-CD4C-9569-BBCC5986633D}" name="Column2" dataDxfId="9">
@@ -2014,7 +2020,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BFDCCA1F-E576-BE4F-AA28-85F02E867175}" name="Table7" displayName="Table7" ref="E40:F67" totalsRowShown="0">
   <autoFilter ref="E40:F67" xr:uid="{E3DFB259-5FDE-CA4D-8DFB-6E893E7430C0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E41:F67">
-    <sortCondition ref="E40:E67"/>
+    <sortCondition descending="1" ref="E40:E67"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{70225ED6-4EBA-BA45-88BF-DE78B29F6418}" name="Column1"/>
@@ -3481,10 +3487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F94A1FA-A4DA-7A4A-A91E-F7469C027059}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="B36" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4005,528 +4011,538 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="17">
-      <c r="A41" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="B41" s="30">
-        <f t="shared" ref="B41:B68" si="2">IFERROR(ROUND(A42,6),"")</f>
-        <v>0.65664199999999995</v>
+      <c r="B41" s="30" t="str">
+        <f t="shared" ref="B41:B62" si="2">IFERROR(ROUND(A42,6),"")</f>
+        <v/>
       </c>
       <c r="C41" s="28" t="str">
-        <f t="shared" ref="C41:C68" si="3">IFERROR(LEFT(RIGHT(A41,LEN(A41)-FIND("'",A41,8)),LEN(A41)-10),"")</f>
-        <v>category_encoders.basen.BaseNEncoder</v>
-      </c>
-      <c r="E41">
-        <v>0.65664199999999995</v>
+        <f t="shared" ref="C41:C63" si="3">IFERROR(LEFT(RIGHT(A41,LEN(A41)-FIND("'",A41,8)),LEN(A41)-10),"")</f>
+        <v/>
+      </c>
+      <c r="E41" t="s">
+        <v>244</v>
       </c>
       <c r="F41" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17">
-      <c r="A42" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B42" s="30" t="str">
+      <c r="A42" s="28" t="s">
+        <v>264</v>
+      </c>
+      <c r="B42" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.62865000000000004</v>
       </c>
       <c r="C42" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E42">
-        <v>0.65664199999999995</v>
+        <v>category_encoders.backward_difference.BackwardDifferenceEncoder</v>
+      </c>
+      <c r="E42" t="s">
+        <v>244</v>
       </c>
       <c r="F42" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17">
-      <c r="A43" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="B43" s="30">
+      <c r="A43" s="28">
+        <v>0.62864971191808094</v>
+      </c>
+      <c r="B43" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C43" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.binary.BinaryEncoder</v>
-      </c>
-      <c r="E43">
-        <v>0.65664199999999995</v>
+        <v/>
+      </c>
+      <c r="E43" t="s">
+        <v>244</v>
       </c>
       <c r="F43" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17">
-      <c r="A44" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B44" s="30" t="str">
+      <c r="A44" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.49974400000000002</v>
       </c>
       <c r="C44" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E44">
-        <v>0.65664199999999995</v>
+        <v>category_encoders.basen.BaseNEncoder</v>
+      </c>
+      <c r="E44" t="s">
+        <v>244</v>
       </c>
       <c r="F44" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17">
-      <c r="A45" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="B45" s="30">
+      <c r="A45" s="28">
+        <v>0.49974420314536599</v>
+      </c>
+      <c r="B45" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C45" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.cat_boost.CatBoostEncoder</v>
-      </c>
-      <c r="E45">
-        <v>0.65664199999999995</v>
+        <v/>
+      </c>
+      <c r="E45" t="s">
+        <v>244</v>
       </c>
       <c r="F45" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17">
-      <c r="A46" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B46" s="30" t="str">
+      <c r="A46" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B46" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.49974400000000002</v>
       </c>
       <c r="C46" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E46">
-        <v>0.65664199999999995</v>
+        <v>category_encoders.binary.BinaryEncoder</v>
+      </c>
+      <c r="E46" t="s">
+        <v>244</v>
       </c>
       <c r="F46" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17">
-      <c r="A47" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="B47" s="30">
+      <c r="A47" s="28">
+        <v>0.49974420314536599</v>
+      </c>
+      <c r="B47" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C47" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.hashing.HashingEncoder</v>
-      </c>
-      <c r="E47">
-        <v>0.65664199999999995</v>
+        <v/>
+      </c>
+      <c r="E47" t="s">
+        <v>244</v>
       </c>
       <c r="F47" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17">
-      <c r="A48" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B48" s="30" t="str">
+      <c r="A48" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.64242900000000003</v>
       </c>
       <c r="C48" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E48">
-        <v>0.65664199999999995</v>
+        <v>category_encoders.cat_boost.CatBoostEncoder</v>
+      </c>
+      <c r="E48" t="s">
+        <v>244</v>
       </c>
       <c r="F48" t="s">
-        <v>230</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17">
-      <c r="A49" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="B49" s="30">
+      <c r="A49" s="28">
+        <v>0.64242881727466405</v>
+      </c>
+      <c r="B49" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C49" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.helmert.HelmertEncoder</v>
-      </c>
-      <c r="E49">
-        <v>0.65664199999999995</v>
+        <v/>
+      </c>
+      <c r="E49" t="s">
+        <v>244</v>
       </c>
       <c r="F49" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17">
-      <c r="A50" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B50" s="30" t="str">
+      <c r="A50" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="B50" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.41559400000000002</v>
       </c>
       <c r="C50" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E50">
-        <v>0.65664199999999995</v>
+        <v>category_encoders.hashing.HashingEncoder</v>
+      </c>
+      <c r="E50" t="s">
+        <v>244</v>
       </c>
       <c r="F50" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17">
-      <c r="A51" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="B51" s="30">
+      <c r="A51" s="28">
+        <v>0.41559417765455903</v>
+      </c>
+      <c r="B51" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C51" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.james_stein.JamesSteinEncoder</v>
-      </c>
-      <c r="E51">
-        <v>0.65664199999999995</v>
+        <v/>
+      </c>
+      <c r="E51" t="s">
+        <v>244</v>
       </c>
       <c r="F51" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17">
-      <c r="A52" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B52" s="30" t="str">
+      <c r="A52" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="B52" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.66555799999999998</v>
       </c>
       <c r="C52" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E52">
-        <v>0.65664199999999995</v>
+        <v>category_encoders.helmert.HelmertEncoder</v>
+      </c>
+      <c r="E52" t="s">
+        <v>244</v>
       </c>
       <c r="F52" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17">
-      <c r="A53" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" s="30">
+      <c r="A53" s="28">
+        <v>0.66555757328114695</v>
+      </c>
+      <c r="B53" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C53" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.one_hot.OneHotEncoder</v>
-      </c>
-      <c r="E53">
-        <v>0.65664199999999995</v>
+        <v/>
+      </c>
+      <c r="E53" t="s">
+        <v>244</v>
       </c>
       <c r="F53" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17">
-      <c r="A54" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B54" s="30" t="str">
+      <c r="A54" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="B54" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.64254100000000003</v>
       </c>
       <c r="C54" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>category_encoders.james_stein.JamesSteinEncoder</v>
       </c>
       <c r="E54">
-        <v>0.65664199999999995</v>
+        <v>0.66555799999999998</v>
       </c>
       <c r="F54" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17">
-      <c r="A55" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="B55" s="30">
+      <c r="A55" s="28">
+        <v>0.64254063813065099</v>
+      </c>
+      <c r="B55" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C55" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.leave_one_out.LeaveOneOutEncoder</v>
-      </c>
-      <c r="E55" t="s">
-        <v>244</v>
+        <v/>
+      </c>
+      <c r="E55">
+        <v>0.65323699999999996</v>
       </c>
       <c r="F55" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17">
-      <c r="A56" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B56" s="30" t="str">
+      <c r="A56" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B56" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.64572200000000002</v>
       </c>
       <c r="C56" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E56" t="s">
-        <v>244</v>
+        <v>category_encoders.one_hot.OneHotEncoder</v>
+      </c>
+      <c r="E56">
+        <v>0.65315000000000001</v>
       </c>
       <c r="F56" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17">
-      <c r="A57" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="B57" s="30">
+      <c r="A57" s="28">
+        <v>0.64572209931566404</v>
+      </c>
+      <c r="B57" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C57" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.m_estimate.MEstimateEncoder</v>
-      </c>
-      <c r="E57" t="s">
-        <v>244</v>
+        <v/>
+      </c>
+      <c r="E57">
+        <v>0.65220999999999996</v>
       </c>
       <c r="F57" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17">
-      <c r="A58" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B58" s="30" t="str">
+      <c r="A58" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="B58" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.63551899999999995</v>
       </c>
       <c r="C58" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E58" t="s">
-        <v>244</v>
+        <v>category_encoders.leave_one_out.LeaveOneOutEncoder</v>
+      </c>
+      <c r="E58">
+        <v>0.64572200000000002</v>
       </c>
       <c r="F58" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17">
-      <c r="A59" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="B59" s="30">
+      <c r="A59" s="28">
+        <v>0.63551903729822401</v>
+      </c>
+      <c r="B59" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C59" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.ordinal.OrdinalEncoder</v>
-      </c>
-      <c r="E59" t="s">
-        <v>244</v>
+        <v/>
+      </c>
+      <c r="E59">
+        <v>0.64254100000000003</v>
       </c>
       <c r="F59" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17">
-      <c r="A60" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B60" s="30" t="str">
+      <c r="A60" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="B60" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.65220999999999996</v>
       </c>
       <c r="C60" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E60" t="s">
-        <v>244</v>
+        <v>category_encoders.m_estimate.MEstimateEncoder</v>
+      </c>
+      <c r="E60">
+        <v>0.64242900000000003</v>
       </c>
       <c r="F60" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17">
-      <c r="A61" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="B61" s="30">
+      <c r="A61" s="28">
+        <v>0.65220993655674198</v>
+      </c>
+      <c r="B61" s="30" t="str">
         <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v/>
       </c>
       <c r="C61" s="28" t="str">
         <f t="shared" si="3"/>
-        <v>category_encoders.polynomial.PolynomialEncoder</v>
-      </c>
-      <c r="E61" t="s">
-        <v>244</v>
+        <v/>
+      </c>
+      <c r="E61">
+        <v>0.63952299999999995</v>
       </c>
       <c r="F61" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17">
-      <c r="A62" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B62" s="30" t="str">
+      <c r="A62" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B62" s="30">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0.426564</v>
       </c>
       <c r="C62" s="28" t="str">
         <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E62" t="s">
-        <v>244</v>
+        <v>category_encoders.ordinal.OrdinalEncoder</v>
+      </c>
+      <c r="E62">
+        <v>0.63551899999999995</v>
       </c>
       <c r="F62" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="17">
-      <c r="A63" s="28" t="s">
-        <v>223</v>
-      </c>
-      <c r="B63" s="30">
-        <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="34">
+      <c r="A63" s="28">
+        <v>0.42656365802734503</v>
+      </c>
+      <c r="B63" s="30" t="str">
+        <f t="shared" ref="B63:B69" si="4">IFERROR(ROUND(A64,6),"")</f>
+        <v/>
       </c>
       <c r="C63" s="28" t="str">
         <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="E63">
+        <v>0.62865000000000004</v>
+      </c>
+      <c r="F63" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="17">
+      <c r="A64" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="B64" s="30">
+        <f t="shared" si="4"/>
+        <v>0.63952299999999995</v>
+      </c>
+      <c r="C64" s="28" t="str">
+        <f t="shared" ref="C64:C66" si="5">IFERROR(LEFT(RIGHT(A64,LEN(A64)-FIND("'",A64,8)),LEN(A64)-10),"")</f>
         <v>category_encoders.sum_coding.SumEncoder</v>
       </c>
-      <c r="E63" t="s">
-        <v>244</v>
-      </c>
-      <c r="F63" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="17">
-      <c r="A64" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B64" s="30" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C64" s="28" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E64" t="s">
-        <v>244</v>
+      <c r="E64">
+        <v>0.49974400000000002</v>
       </c>
       <c r="F64" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17">
-      <c r="A65" s="28" t="s">
+      <c r="A65" s="28">
+        <v>0.63952296378973394</v>
+      </c>
+      <c r="B65" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C65" s="28" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E65">
+        <v>0.49974400000000002</v>
+      </c>
+      <c r="F65" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="17">
+      <c r="A66" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="B65" s="30">
-        <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
-      </c>
-      <c r="C65" s="28" t="str">
-        <f t="shared" si="3"/>
+      <c r="B66" s="30">
+        <f t="shared" si="4"/>
+        <v>0.65315000000000001</v>
+      </c>
+      <c r="C66" s="28" t="str">
+        <f t="shared" si="5"/>
         <v>category_encoders.target_encoder.TargetEncoder</v>
       </c>
-      <c r="E65" t="s">
-        <v>244</v>
-      </c>
-      <c r="F65" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="17">
-      <c r="A66" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B66" s="30" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="C66" s="28" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="E66" t="s">
-        <v>244</v>
+      <c r="E66">
+        <v>0.426564</v>
       </c>
       <c r="F66" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17">
-      <c r="A67" s="28" t="s">
+      <c r="A67" s="28">
+        <v>0.65314952090281297</v>
+      </c>
+      <c r="B67" s="30" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="C67" s="28" t="str">
+        <f t="shared" ref="C67:C69" si="6">IFERROR(LEFT(RIGHT(A67,LEN(A67)-FIND("'",A67,8)),LEN(A67)-10),"")</f>
+        <v/>
+      </c>
+      <c r="E67">
+        <v>0.41559400000000002</v>
+      </c>
+      <c r="F67" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="17">
+      <c r="A68" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="B67" s="30">
-        <f t="shared" si="2"/>
-        <v>0.65664199999999995</v>
-      </c>
-      <c r="C67" s="28" t="str">
-        <f t="shared" si="3"/>
+      <c r="B68" s="30">
+        <f t="shared" si="4"/>
+        <v>0.65323699999999996</v>
+      </c>
+      <c r="C68" s="28" t="str">
+        <f t="shared" si="6"/>
         <v>category_encoders.woe.WOEEncoder</v>
       </c>
-      <c r="E67" t="s">
-        <v>244</v>
-      </c>
-      <c r="F67" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="17">
-      <c r="A68" s="28">
-        <v>0.65664176497871896</v>
-      </c>
-      <c r="B68" s="30">
-        <f t="shared" si="2"/>
+    </row>
+    <row r="69" spans="1:6" ht="17">
+      <c r="A69" s="28">
+        <v>0.65323690662962997</v>
+      </c>
+      <c r="B69" s="30">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="C68" s="28" t="str">
-        <f t="shared" si="3"/>
+      <c r="C69" s="28" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
     </row>
@@ -4544,10 +4560,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6ABCD42-C9AE-9443-A5B9-A0E03BC995D4}">
-  <dimension ref="A2:E30"/>
+  <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4633,7 +4649,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19">
+    <row r="9" spans="1:5" ht="18">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -4644,7 +4660,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="19">
+    <row r="10" spans="1:5" ht="18">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -4655,7 +4671,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="19">
+    <row r="11" spans="1:5" ht="18">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -4666,7 +4682,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19">
+    <row r="12" spans="1:5" ht="18">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -4677,7 +4693,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="19">
+    <row r="13" spans="1:5" ht="18">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -4688,7 +4704,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="19">
+    <row r="14" spans="1:5" ht="18">
       <c r="A14" s="1">
         <v>7</v>
       </c>
@@ -4860,7 +4876,6 @@
         <v>3.9302974044397199E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="17"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5341,7 +5356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCD804D-D4BC-DF4B-B369-C04D16475947}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>